<commit_message>
Changed the crossover operator for the GA to properly function even with smaller amounts of packages
</commit_message>
<xml_diff>
--- a/Genetic Algorithm Autom Pack/Experiment Data.xlsx
+++ b/Genetic Algorithm Autom Pack/Experiment Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="31">
   <si>
     <t>Tournament selection</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>Roulette selection</t>
+  </si>
+  <si>
+    <t>Average gaps</t>
+  </si>
+  <si>
+    <t>Most gaps</t>
+  </si>
+  <si>
+    <t>Least gaps</t>
   </si>
 </sst>
 </file>
@@ -486,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O133"/>
+  <dimension ref="A1:R133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="Q69" sqref="Q69"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +518,7 @@
     <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I1" t="s">
         <v>14</v>
       </c>
@@ -517,7 +526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -529,7 +538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -541,7 +550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -553,7 +562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -565,7 +574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -577,7 +586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -589,7 +598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -618,8 +627,17 @@
       <c r="O8" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -649,7 +667,7 @@
         <v>4086</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -679,7 +697,7 @@
         <v>8944</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -709,7 +727,7 @@
         <v>14432</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -739,7 +757,7 @@
         <v>20723</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -769,7 +787,7 @@
         <v>29298</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -799,7 +817,7 @@
         <v>34432</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -829,7 +847,7 @@
         <v>40225</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>

</xml_diff>

<commit_message>
Done with repeating yesterday's test with more data
</commit_message>
<xml_diff>
--- a/Genetic Algorithm Autom Pack/Experiment Data.xlsx
+++ b/Genetic Algorithm Autom Pack/Experiment Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="34">
   <si>
     <t>Tournament selection</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>Least gaps</t>
+  </si>
+  <si>
+    <t>Average A</t>
+  </si>
+  <si>
+    <t>Average B</t>
+  </si>
+  <si>
+    <t>Average C</t>
   </si>
 </sst>
 </file>
@@ -495,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R133"/>
+  <dimension ref="A1:AA133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="E29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:U66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,18 +516,30 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I1" t="s">
         <v>14</v>
       </c>
@@ -526,7 +547,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -538,7 +559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -550,7 +571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -562,7 +583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -574,7 +595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -586,7 +607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -598,7 +619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -636,8 +657,17 @@
       <c r="R8" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -649,13 +679,13 @@
         <v>10</v>
       </c>
       <c r="J9" s="1">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K9" s="1">
-        <v>180</v>
+        <v>228.3</v>
       </c>
       <c r="L9" s="1">
-        <v>227.6</v>
+        <v>196</v>
       </c>
       <c r="M9" s="1">
         <v>468</v>
@@ -666,8 +696,26 @@
       <c r="O9" s="1">
         <v>4086</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P9" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>79.650000000000006</v>
+      </c>
+      <c r="R9" s="1">
+        <v>264</v>
+      </c>
+      <c r="S9" s="1">
+        <v>36.15</v>
+      </c>
+      <c r="T9" s="1">
+        <v>6.15</v>
+      </c>
+      <c r="U9" s="1">
+        <v>19.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -696,8 +744,26 @@
       <c r="O10" s="4">
         <v>8944</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P10" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>60.35</v>
+      </c>
+      <c r="R10" s="1">
+        <v>102</v>
+      </c>
+      <c r="S10" s="1">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="T10" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="U10" s="1">
+        <v>20.55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -726,8 +792,26 @@
       <c r="O11" s="5">
         <v>14432</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P11" s="5">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>40.6</v>
+      </c>
+      <c r="R11" s="5">
+        <v>89</v>
+      </c>
+      <c r="S11" s="5">
+        <v>33.35</v>
+      </c>
+      <c r="T11" s="5">
+        <v>7</v>
+      </c>
+      <c r="U11" s="5">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -756,8 +840,26 @@
       <c r="O12" s="1">
         <v>20723</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P12" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>33.4</v>
+      </c>
+      <c r="R12" s="1">
+        <v>84</v>
+      </c>
+      <c r="S12" s="1">
+        <v>32.9</v>
+      </c>
+      <c r="T12" s="1">
+        <v>7.15</v>
+      </c>
+      <c r="U12" s="1">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -786,8 +888,26 @@
       <c r="O13" s="1">
         <v>29298</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P13" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="R13" s="1">
+        <v>70</v>
+      </c>
+      <c r="S13" s="1">
+        <v>32</v>
+      </c>
+      <c r="T13" s="1">
+        <v>7.95</v>
+      </c>
+      <c r="U13" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -816,8 +936,26 @@
       <c r="O14" s="1">
         <v>34432</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P14" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>14.4</v>
+      </c>
+      <c r="R14" s="1">
+        <v>38</v>
+      </c>
+      <c r="S14" s="1">
+        <v>30.9</v>
+      </c>
+      <c r="T14" s="1">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="U14" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -846,8 +984,26 @@
       <c r="O15" s="1">
         <v>40225</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P15" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="R15" s="1">
+        <v>54</v>
+      </c>
+      <c r="S15" s="1">
+        <v>31.3</v>
+      </c>
+      <c r="T15" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="U15" s="1">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -856,7 +1012,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
@@ -870,7 +1026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>13</v>
       </c>
@@ -884,7 +1040,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
@@ -898,7 +1054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>10</v>
       </c>
@@ -912,7 +1068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>11</v>
       </c>
@@ -926,7 +1082,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -969,8 +1125,26 @@
       <c r="O22" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>10</v>
       </c>
@@ -1013,8 +1187,26 @@
       <c r="O23" s="1">
         <v>13494</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P23" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>59.85</v>
+      </c>
+      <c r="R23" s="1">
+        <v>89</v>
+      </c>
+      <c r="S23" s="1">
+        <v>34.049999999999997</v>
+      </c>
+      <c r="T23" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="U23" s="1">
+        <v>21.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>20</v>
       </c>
@@ -1057,8 +1249,26 @@
       <c r="O24" s="5">
         <v>14204</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24" s="5">
+        <v>6</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>42.05</v>
+      </c>
+      <c r="R24" s="5">
+        <v>102</v>
+      </c>
+      <c r="S24" s="5">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="T24" s="5">
+        <v>6.65</v>
+      </c>
+      <c r="U24" s="5">
+        <v>21.45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>30</v>
       </c>
@@ -1101,8 +1311,26 @@
       <c r="O25" s="4">
         <v>13873</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>43.8</v>
+      </c>
+      <c r="R25" s="1">
+        <v>89</v>
+      </c>
+      <c r="S25" s="1">
+        <v>33.15</v>
+      </c>
+      <c r="T25" s="1">
+        <v>7</v>
+      </c>
+      <c r="U25" s="1">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>40</v>
       </c>
@@ -1128,7 +1356,7 @@
         <v>40</v>
       </c>
       <c r="J26" s="1">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K26" s="1">
         <v>232.94</v>
@@ -1145,8 +1373,26 @@
       <c r="O26" s="1">
         <v>13626</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>54</v>
+      </c>
+      <c r="R26" s="1">
+        <v>81</v>
+      </c>
+      <c r="S26" s="1">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="T26" s="1">
+        <v>8</v>
+      </c>
+      <c r="U26" s="1">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>50</v>
       </c>
@@ -1172,7 +1418,7 @@
         <v>50</v>
       </c>
       <c r="J27" s="1">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K27" s="1">
         <v>232.1</v>
@@ -1189,8 +1435,26 @@
       <c r="O27" s="1">
         <v>13218</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27" s="1">
+        <v>42</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>63.8</v>
+      </c>
+      <c r="R27" s="1">
+        <v>106</v>
+      </c>
+      <c r="S27" s="1">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="T27" s="1">
+        <v>7.15</v>
+      </c>
+      <c r="U27" s="1">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>60</v>
       </c>
@@ -1216,7 +1480,7 @@
         <v>60</v>
       </c>
       <c r="J28" s="1">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K28" s="1">
         <v>231.2</v>
@@ -1233,8 +1497,26 @@
       <c r="O28" s="1">
         <v>15103</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28" s="1">
+        <v>38</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>54.85</v>
+      </c>
+      <c r="R28" s="1">
+        <v>89</v>
+      </c>
+      <c r="S28" s="1">
+        <v>31.7</v>
+      </c>
+      <c r="T28" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="U28" s="1">
+        <v>21.05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1243,7 +1525,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>12</v>
       </c>
@@ -1257,7 +1539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>13</v>
       </c>
@@ -1271,7 +1553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>9</v>
       </c>
@@ -1285,7 +1567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>8</v>
       </c>
@@ -1299,7 +1581,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>10</v>
       </c>
@@ -1313,7 +1595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>16</v>
       </c>
@@ -1356,8 +1638,26 @@
       <c r="O35" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>0</v>
       </c>
@@ -1383,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="1">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="K36" s="1">
         <v>219.4</v>
@@ -1400,8 +1700,26 @@
       <c r="O36" s="1">
         <v>14323</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36" s="1">
+        <v>93</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>121.1</v>
+      </c>
+      <c r="R36" s="1">
+        <v>148</v>
+      </c>
+      <c r="S36" s="1">
+        <v>31.3</v>
+      </c>
+      <c r="T36" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="U36" s="1">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>1</v>
       </c>
@@ -1427,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="J37" s="1">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="K37" s="1">
         <v>220.12</v>
@@ -1444,8 +1762,26 @@
       <c r="O37" s="1">
         <v>14738</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37" s="1">
+        <v>81</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>119.85</v>
+      </c>
+      <c r="R37" s="1">
+        <v>141</v>
+      </c>
+      <c r="S37" s="1">
+        <v>31.2</v>
+      </c>
+      <c r="T37" s="1">
+        <v>9.35</v>
+      </c>
+      <c r="U37" s="1">
+        <v>17.649999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>2</v>
       </c>
@@ -1488,8 +1824,26 @@
       <c r="O38" s="5">
         <v>15346</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P38" s="5">
+        <v>6</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>36.049999999999997</v>
+      </c>
+      <c r="R38" s="5">
+        <v>70</v>
+      </c>
+      <c r="S38" s="5">
+        <v>33.1</v>
+      </c>
+      <c r="T38" s="5">
+        <v>7.3</v>
+      </c>
+      <c r="U38" s="5">
+        <v>21.45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>3</v>
       </c>
@@ -1521,7 +1875,7 @@
         <v>234.12</v>
       </c>
       <c r="L39" s="4">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="M39" s="4">
         <v>1667</v>
@@ -1532,8 +1886,26 @@
       <c r="O39" s="4">
         <v>14234</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P39" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>49</v>
+      </c>
+      <c r="R39" s="1">
+        <v>86</v>
+      </c>
+      <c r="S39" s="1">
+        <v>34.549999999999997</v>
+      </c>
+      <c r="T39" s="1">
+        <v>5.85</v>
+      </c>
+      <c r="U39" s="1">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>4</v>
       </c>
@@ -1565,7 +1937,7 @@
         <v>235.58</v>
       </c>
       <c r="L40" s="1">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M40" s="1">
         <v>1626</v>
@@ -1576,8 +1948,26 @@
       <c r="O40" s="1">
         <v>13722</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P40" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>34.549999999999997</v>
+      </c>
+      <c r="R40" s="1">
+        <v>89</v>
+      </c>
+      <c r="S40" s="1">
+        <v>32.65</v>
+      </c>
+      <c r="T40" s="1">
+        <v>7.55</v>
+      </c>
+      <c r="U40" s="1">
+        <v>21.55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1595,7 +1985,7 @@
         <v>234.78</v>
       </c>
       <c r="L41" s="1">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M41" s="1">
         <v>1630</v>
@@ -1606,8 +1996,26 @@
       <c r="O41" s="1">
         <v>13433</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P41" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>48.7</v>
+      </c>
+      <c r="R41" s="1">
+        <v>92</v>
+      </c>
+      <c r="S41" s="1">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="T41" s="1">
+        <v>6.15</v>
+      </c>
+      <c r="U41" s="1">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1623,7 +2031,7 @@
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>12</v>
       </c>
@@ -1637,7 +2045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>13</v>
       </c>
@@ -1651,7 +2059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>9</v>
       </c>
@@ -1665,7 +2073,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>8</v>
       </c>
@@ -1679,7 +2087,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>11</v>
       </c>
@@ -1693,7 +2101,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>17</v>
       </c>
@@ -1736,8 +2144,26 @@
       <c r="O48" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>0.01</v>
       </c>
@@ -1780,8 +2206,14 @@
       <c r="O49" s="1">
         <v>15801</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>0.02</v>
       </c>
@@ -1812,8 +2244,14 @@
       <c r="O50" s="1">
         <v>15504</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>0.05</v>
       </c>
@@ -1844,8 +2282,14 @@
       <c r="O51" s="5">
         <v>14947</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>3</v>
       </c>
@@ -1876,8 +2320,14 @@
       <c r="O52" s="4">
         <v>14040</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>4</v>
       </c>
@@ -1908,8 +2358,14 @@
       <c r="O53" s="1">
         <v>14263</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1927,32 +2383,32 @@
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I56" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I57" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I58" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I59" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I60" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I61" s="1" t="s">
         <v>19</v>
       </c>
@@ -1975,7 +2431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I62" s="1">
         <v>0</v>
       </c>
@@ -1998,7 +2454,7 @@
         <v>14432</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I63" s="1">
         <v>0.01</v>
       </c>
@@ -2021,7 +2477,7 @@
         <v>16416</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I64" s="1">
         <v>0.02</v>
       </c>
@@ -2044,7 +2500,7 @@
         <v>14831</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I65" s="1">
         <v>0.03</v>
       </c>
@@ -2067,7 +2523,7 @@
         <v>14979</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I66" s="1">
         <v>0.04</v>
       </c>
@@ -2090,7 +2546,7 @@
         <v>13674</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
@@ -2099,55 +2555,55 @@
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="O69" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I70" s="3" t="s">
+      <c r="O70" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>23</v>
       </c>
-      <c r="I71" t="s">
+      <c r="O71" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>9</v>
       </c>
-      <c r="I72" t="s">
+      <c r="O72" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>10</v>
       </c>
-      <c r="I73" t="s">
+      <c r="O73" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>11</v>
       </c>
-      <c r="I74" t="s">
+      <c r="O74" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>7</v>
       </c>
@@ -2169,29 +2625,65 @@
       <c r="G75" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="H75" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="I75" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J75" s="1" t="s">
+      <c r="P75" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K75" s="1" t="s">
+      <c r="Q75" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L75" s="1" t="s">
+      <c r="R75" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M75" s="1" t="s">
+      <c r="S75" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N75" s="1" t="s">
+      <c r="T75" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O75" s="1" t="s">
+      <c r="U75" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="V75" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W75" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X75" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y75" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z75" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA75" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>10</v>
       </c>
@@ -2213,29 +2705,29 @@
       <c r="G76" s="1">
         <v>4112</v>
       </c>
-      <c r="I76" s="1">
+      <c r="O76" s="1">
         <v>10</v>
       </c>
-      <c r="J76" s="4">
+      <c r="P76" s="4">
         <v>235</v>
       </c>
-      <c r="K76" s="4">
+      <c r="Q76" s="4">
         <v>227.84</v>
       </c>
-      <c r="L76" s="4">
+      <c r="R76" s="4">
         <v>195</v>
       </c>
-      <c r="M76" s="4">
+      <c r="S76" s="4">
         <v>489</v>
       </c>
-      <c r="N76" s="4">
+      <c r="T76" s="4">
         <v>2348.2600000000002</v>
       </c>
-      <c r="O76" s="4">
+      <c r="U76" s="4">
         <v>4060</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>20</v>
       </c>
@@ -2257,29 +2749,29 @@
       <c r="G77" s="4">
         <v>8248</v>
       </c>
-      <c r="I77" s="1">
+      <c r="O77" s="1">
         <v>20</v>
       </c>
-      <c r="J77" s="4">
+      <c r="P77" s="4">
         <v>239</v>
       </c>
-      <c r="K77" s="4">
+      <c r="Q77" s="4">
         <v>232.08</v>
       </c>
-      <c r="L77" s="4">
+      <c r="R77" s="4">
         <v>222</v>
       </c>
-      <c r="M77" s="4">
+      <c r="S77" s="4">
         <v>894</v>
       </c>
-      <c r="N77" s="4">
+      <c r="T77" s="4">
         <v>2228.7399999999998</v>
       </c>
-      <c r="O77" s="4">
+      <c r="U77" s="4">
         <v>7796</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>35</v>
       </c>
@@ -2301,29 +2793,29 @@
       <c r="G78" s="9">
         <v>14475</v>
       </c>
-      <c r="I78" s="1">
+      <c r="O78" s="1">
         <v>35</v>
       </c>
-      <c r="J78" s="10">
+      <c r="P78" s="10">
         <v>240</v>
       </c>
-      <c r="K78" s="10">
+      <c r="Q78" s="10">
         <v>235.14</v>
       </c>
-      <c r="L78" s="10">
+      <c r="R78" s="10">
         <v>228</v>
       </c>
-      <c r="M78" s="10">
+      <c r="S78" s="10">
         <v>1602</v>
       </c>
-      <c r="N78" s="10">
+      <c r="T78" s="10">
         <v>2348.84</v>
       </c>
-      <c r="O78" s="10">
+      <c r="U78" s="10">
         <v>16304</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>50</v>
       </c>
@@ -2345,29 +2837,29 @@
       <c r="G79" s="1">
         <v>20120</v>
       </c>
-      <c r="I79" s="1">
+      <c r="O79" s="1">
         <v>50</v>
       </c>
-      <c r="J79" s="4">
+      <c r="P79" s="4">
         <v>240</v>
       </c>
-      <c r="K79" s="4">
+      <c r="Q79" s="4">
         <v>236.34</v>
       </c>
-      <c r="L79" s="4">
+      <c r="R79" s="4">
         <v>228</v>
       </c>
-      <c r="M79" s="4">
+      <c r="S79" s="4">
         <v>2563</v>
       </c>
-      <c r="N79" s="4">
+      <c r="T79" s="4">
         <v>3610.92</v>
       </c>
-      <c r="O79" s="4">
+      <c r="U79" s="4">
         <v>21967</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>70</v>
       </c>
@@ -2389,29 +2881,29 @@
       <c r="G80" s="1">
         <v>27410</v>
       </c>
-      <c r="I80" s="1">
+      <c r="O80" s="1">
         <v>70</v>
       </c>
-      <c r="J80" s="4">
+      <c r="P80" s="4">
         <v>240</v>
       </c>
-      <c r="K80" s="4">
+      <c r="Q80" s="4">
         <v>237.34</v>
       </c>
-      <c r="L80" s="4">
+      <c r="R80" s="4">
         <v>231</v>
       </c>
-      <c r="M80" s="4">
+      <c r="S80" s="4">
         <v>3490</v>
       </c>
-      <c r="N80" s="4">
+      <c r="T80" s="4">
         <v>3920.18</v>
       </c>
-      <c r="O80" s="4">
+      <c r="U80" s="4">
         <v>4766</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>85</v>
       </c>
@@ -2433,29 +2925,29 @@
       <c r="G81" s="1">
         <v>4639</v>
       </c>
-      <c r="I81" s="1">
+      <c r="O81" s="1">
         <v>85</v>
       </c>
-      <c r="J81" s="4">
+      <c r="P81" s="4">
         <v>240</v>
       </c>
-      <c r="K81" s="4">
+      <c r="Q81" s="4">
         <v>237.96</v>
       </c>
-      <c r="L81" s="4">
+      <c r="R81" s="4">
         <v>234</v>
       </c>
-      <c r="M81" s="4">
+      <c r="S81" s="4">
         <v>4322</v>
       </c>
-      <c r="N81" s="4">
+      <c r="T81" s="4">
         <v>4803.58</v>
       </c>
-      <c r="O81" s="4">
+      <c r="U81" s="4">
         <v>5116</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>100</v>
       </c>
@@ -2477,91 +2969,91 @@
       <c r="G82" s="1">
         <v>5552</v>
       </c>
-      <c r="I82" s="1">
+      <c r="O82" s="1">
         <v>100</v>
       </c>
-      <c r="J82" s="4">
+      <c r="P82" s="4">
         <v>240</v>
       </c>
-      <c r="K82" s="4">
+      <c r="Q82" s="4">
         <v>238.28</v>
       </c>
-      <c r="L82" s="4">
+      <c r="R82" s="4">
         <v>236</v>
       </c>
-      <c r="M82" s="4">
+      <c r="S82" s="4">
         <v>4950</v>
       </c>
-      <c r="N82" s="4">
+      <c r="T82" s="4">
         <v>5370.44</v>
       </c>
-      <c r="O82" s="4">
+      <c r="U82" s="4">
         <v>6045</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I83" s="1">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O83" s="1">
         <v>125</v>
       </c>
-      <c r="J83" s="4">
+      <c r="P83" s="4">
         <v>240</v>
       </c>
-      <c r="K83" s="4">
+      <c r="Q83" s="4">
         <v>238.62</v>
       </c>
-      <c r="L83" s="4">
+      <c r="R83" s="4">
         <v>238</v>
       </c>
-      <c r="M83" s="4">
+      <c r="S83" s="4">
         <v>6215</v>
       </c>
-      <c r="N83" s="4">
+      <c r="T83" s="4">
         <v>6419.5</v>
       </c>
-      <c r="O83" s="4">
+      <c r="U83" s="4">
         <v>6723</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I84" s="1"/>
-      <c r="J84" s="4"/>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O84" s="1"/>
+      <c r="P84" s="4"/>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>18</v>
       </c>
-      <c r="I85" s="3" t="s">
+      <c r="O85" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>9</v>
       </c>
-      <c r="I86" t="s">
+      <c r="O86" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>10</v>
       </c>
-      <c r="I87" t="s">
+      <c r="O87" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>11</v>
       </c>
-      <c r="I88" t="s">
+      <c r="O88" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>24</v>
       </c>
@@ -2583,11 +3075,29 @@
       <c r="G89" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I89" t="s">
+      <c r="H89" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O89" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>5</v>
       </c>
@@ -2609,29 +3119,47 @@
       <c r="G90" s="1">
         <v>13818</v>
       </c>
-      <c r="I90" s="1" t="s">
+      <c r="O90" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J90" s="1" t="s">
+      <c r="P90" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K90" s="1" t="s">
+      <c r="Q90" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L90" s="1" t="s">
+      <c r="R90" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M90" s="1" t="s">
+      <c r="S90" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N90" s="1" t="s">
+      <c r="T90" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O90" s="1" t="s">
+      <c r="U90" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="V90" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W90" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X90" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y90" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z90" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA90" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>10</v>
       </c>
@@ -2653,29 +3181,29 @@
       <c r="G91" s="4">
         <v>14075</v>
       </c>
-      <c r="I91" s="1">
+      <c r="O91" s="1">
         <v>0</v>
       </c>
-      <c r="J91" s="4">
+      <c r="P91" s="4">
         <v>221</v>
       </c>
-      <c r="K91" s="4">
+      <c r="Q91" s="4">
         <v>212.5</v>
       </c>
-      <c r="L91" s="4">
+      <c r="R91" s="4">
         <v>206</v>
       </c>
-      <c r="M91" s="4">
+      <c r="S91" s="4">
         <v>11275</v>
       </c>
-      <c r="N91" s="4">
+      <c r="T91" s="4">
         <v>12818.1</v>
       </c>
-      <c r="O91" s="4">
+      <c r="U91" s="4">
         <v>15476</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>20</v>
       </c>
@@ -2697,29 +3225,29 @@
       <c r="G92" s="9">
         <v>13736</v>
       </c>
-      <c r="I92" s="1">
+      <c r="O92" s="1">
         <v>1</v>
       </c>
-      <c r="J92" s="4">
+      <c r="P92" s="4">
         <v>221</v>
       </c>
-      <c r="K92" s="4">
+      <c r="Q92" s="4">
         <v>212.08</v>
       </c>
-      <c r="L92" s="4">
+      <c r="R92" s="4">
         <v>206</v>
       </c>
-      <c r="M92" s="4">
+      <c r="S92" s="4">
         <v>11621</v>
       </c>
-      <c r="N92" s="4">
+      <c r="T92" s="4">
         <v>12963.76</v>
       </c>
-      <c r="O92" s="4">
+      <c r="U92" s="4">
         <v>14157</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>30</v>
       </c>
@@ -2741,29 +3269,29 @@
       <c r="G93" s="1">
         <v>14517</v>
       </c>
-      <c r="I93" s="4">
+      <c r="O93" s="4">
         <v>2</v>
       </c>
-      <c r="J93" s="10">
+      <c r="P93" s="10">
         <v>238</v>
       </c>
-      <c r="K93" s="10">
+      <c r="Q93" s="10">
         <v>234.66</v>
       </c>
-      <c r="L93" s="10">
+      <c r="R93" s="10">
         <v>227</v>
       </c>
-      <c r="M93" s="10">
+      <c r="S93" s="10">
         <v>1648</v>
       </c>
-      <c r="N93" s="10">
+      <c r="T93" s="10">
         <v>2779.2</v>
       </c>
-      <c r="O93" s="10">
+      <c r="U93" s="10">
         <v>13710</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>40</v>
       </c>
@@ -2785,29 +3313,29 @@
       <c r="G94" s="1">
         <v>14192</v>
       </c>
-      <c r="I94" s="1">
+      <c r="O94" s="1">
         <v>3</v>
       </c>
-      <c r="J94" s="4">
+      <c r="P94" s="4">
         <v>240</v>
       </c>
-      <c r="K94" s="4">
+      <c r="Q94" s="4">
         <v>233.92</v>
       </c>
-      <c r="L94" s="4">
+      <c r="R94" s="4">
         <v>228</v>
       </c>
-      <c r="M94" s="4">
+      <c r="S94" s="4">
         <v>1663</v>
       </c>
-      <c r="N94" s="4">
+      <c r="T94" s="4">
         <v>3025.76</v>
       </c>
-      <c r="O94" s="4">
+      <c r="U94" s="4">
         <v>14264</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>50</v>
       </c>
@@ -2829,89 +3357,89 @@
       <c r="G95" s="1">
         <v>13896</v>
       </c>
-      <c r="I95" s="1">
+      <c r="O95" s="1">
         <v>4</v>
       </c>
-      <c r="J95" s="4">
+      <c r="P95" s="4">
         <v>239</v>
       </c>
-      <c r="K95" s="4">
+      <c r="Q95" s="4">
         <v>235.42</v>
       </c>
-      <c r="L95" s="4">
+      <c r="R95" s="4">
         <v>228</v>
       </c>
-      <c r="M95" s="4">
+      <c r="S95" s="4">
         <v>1648</v>
       </c>
-      <c r="N95" s="4">
+      <c r="T95" s="4">
         <v>2489.08</v>
       </c>
-      <c r="O95" s="4">
+      <c r="U95" s="4">
         <v>13873</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I96" s="1">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O96" s="1">
         <v>5</v>
       </c>
-      <c r="J96" s="4">
+      <c r="P96" s="4">
         <v>239</v>
       </c>
-      <c r="K96" s="4">
+      <c r="Q96" s="4">
         <v>235.14</v>
       </c>
-      <c r="L96" s="4">
+      <c r="R96" s="4">
         <v>229</v>
       </c>
-      <c r="M96" s="4">
+      <c r="S96" s="4">
         <v>1592</v>
       </c>
-      <c r="N96" s="4">
+      <c r="T96" s="4">
         <v>2041.64</v>
       </c>
-      <c r="O96" s="4">
+      <c r="U96" s="4">
         <v>13770</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>18</v>
       </c>
-      <c r="I98" s="3" t="s">
+      <c r="O98" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>9</v>
       </c>
-      <c r="I99" t="s">
+      <c r="O99" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>25</v>
       </c>
-      <c r="I100" t="s">
+      <c r="O100" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>10</v>
       </c>
-      <c r="I101" t="s">
+      <c r="O101" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>16</v>
       </c>
@@ -2933,11 +3461,29 @@
       <c r="G102" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I102" t="s">
+      <c r="H102" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O102" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>0</v>
       </c>
@@ -2959,29 +3505,47 @@
       <c r="G103" s="1">
         <v>13119</v>
       </c>
-      <c r="I103" s="1" t="s">
+      <c r="O103" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J103" s="1" t="s">
+      <c r="P103" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K103" s="1" t="s">
+      <c r="Q103" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L103" s="1" t="s">
+      <c r="R103" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M103" s="1" t="s">
+      <c r="S103" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N103" s="1" t="s">
+      <c r="T103" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O103" s="1" t="s">
+      <c r="U103" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="V103" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W103" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X103" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y103" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z103" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA103" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>1</v>
       </c>
@@ -3003,29 +3567,29 @@
       <c r="G104" s="1">
         <v>12599</v>
       </c>
-      <c r="I104" s="1">
+      <c r="O104" s="1">
         <v>0.01</v>
       </c>
-      <c r="J104" s="4">
+      <c r="P104" s="4">
         <v>236</v>
       </c>
-      <c r="K104" s="4">
+      <c r="Q104" s="4">
         <v>227.12</v>
       </c>
-      <c r="L104" s="4">
+      <c r="R104" s="4">
         <v>214</v>
       </c>
-      <c r="M104" s="4">
+      <c r="S104" s="4">
         <v>2318</v>
       </c>
-      <c r="N104" s="4">
+      <c r="T104" s="4">
         <v>12114.14</v>
       </c>
-      <c r="O104" s="4">
+      <c r="U104" s="4">
         <v>18036</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>2</v>
       </c>
@@ -3047,29 +3611,29 @@
       <c r="G105" s="9">
         <v>14243</v>
       </c>
-      <c r="I105" s="1">
+      <c r="O105" s="1">
         <v>0.03</v>
       </c>
-      <c r="J105" s="4">
+      <c r="P105" s="4">
         <v>240</v>
       </c>
-      <c r="K105" s="4">
+      <c r="Q105" s="4">
         <v>233.72</v>
       </c>
-      <c r="L105" s="4">
+      <c r="R105" s="4">
         <v>227</v>
       </c>
-      <c r="M105" s="4">
+      <c r="S105" s="4">
         <v>1814</v>
       </c>
-      <c r="N105" s="4">
+      <c r="T105" s="4">
         <v>3470.2</v>
       </c>
-      <c r="O105" s="4">
+      <c r="U105" s="4">
         <v>17093</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>3</v>
       </c>
@@ -3091,29 +3655,29 @@
       <c r="G106" s="4">
         <v>14336</v>
       </c>
-      <c r="I106" s="4">
+      <c r="O106" s="4">
         <v>0.05</v>
       </c>
-      <c r="J106" s="10">
+      <c r="P106" s="10">
         <v>240</v>
       </c>
-      <c r="K106" s="10">
+      <c r="Q106" s="10">
         <v>234.36</v>
       </c>
-      <c r="L106" s="10">
+      <c r="R106" s="10">
         <v>228</v>
       </c>
-      <c r="M106" s="10">
+      <c r="S106" s="10">
         <v>1722</v>
       </c>
-      <c r="N106" s="10">
+      <c r="T106" s="10">
         <v>3150.68</v>
       </c>
-      <c r="O106" s="10">
+      <c r="U106" s="10">
         <v>16023</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>4</v>
       </c>
@@ -3135,29 +3699,29 @@
       <c r="G107" s="1">
         <v>13385</v>
       </c>
-      <c r="I107" s="1">
+      <c r="O107" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J107" s="4">
+      <c r="P107" s="4">
         <v>239</v>
       </c>
-      <c r="K107" s="4">
+      <c r="Q107" s="4">
         <v>234.32</v>
       </c>
-      <c r="L107" s="4">
+      <c r="R107" s="4">
         <v>228</v>
       </c>
-      <c r="M107" s="4">
+      <c r="S107" s="4">
         <v>1721</v>
       </c>
-      <c r="N107" s="4">
+      <c r="T107" s="4">
         <v>2648.64</v>
       </c>
-      <c r="O107" s="4">
+      <c r="U107" s="4">
         <v>14477</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>5</v>
       </c>
@@ -3179,89 +3743,89 @@
       <c r="G108" s="1">
         <v>15379</v>
       </c>
-      <c r="I108" s="1">
+      <c r="O108" s="1">
         <v>0.1</v>
       </c>
-      <c r="J108" s="4">
+      <c r="P108" s="4">
         <v>238</v>
       </c>
-      <c r="K108" s="4">
+      <c r="Q108" s="4">
         <v>233.52</v>
       </c>
-      <c r="L108" s="4">
+      <c r="R108" s="4">
         <v>228</v>
       </c>
-      <c r="M108" s="4">
+      <c r="S108" s="4">
         <v>1607</v>
       </c>
-      <c r="N108" s="4">
+      <c r="T108" s="4">
         <v>3165.94</v>
       </c>
-      <c r="O108" s="4">
+      <c r="U108" s="4">
         <v>13711</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I109" s="1">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O109" s="1">
         <v>0.15</v>
       </c>
-      <c r="J109" s="4">
+      <c r="P109" s="4">
         <v>238</v>
       </c>
-      <c r="K109" s="4">
+      <c r="Q109" s="4">
         <v>233.94</v>
       </c>
-      <c r="L109" s="4">
+      <c r="R109" s="4">
         <v>226</v>
       </c>
-      <c r="M109" s="4">
+      <c r="S109" s="4">
         <v>1549</v>
       </c>
-      <c r="N109" s="4">
+      <c r="T109" s="4">
         <v>1964.26</v>
       </c>
-      <c r="O109" s="4">
+      <c r="U109" s="4">
         <v>14596</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>18</v>
       </c>
-      <c r="I111" s="3" t="s">
+      <c r="O111" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>9</v>
       </c>
-      <c r="I112" t="s">
+      <c r="O112" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>25</v>
       </c>
-      <c r="I113" t="s">
+      <c r="O113" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>11</v>
       </c>
-      <c r="I114" t="s">
+      <c r="O114" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>17</v>
       </c>
@@ -3283,11 +3847,29 @@
       <c r="G115" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I115" t="s">
+      <c r="H115" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L115" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O115" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>0.01</v>
       </c>
@@ -3309,29 +3891,47 @@
       <c r="G116" s="1">
         <v>14688</v>
       </c>
-      <c r="I116" s="1" t="s">
+      <c r="O116" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J116" s="1" t="s">
+      <c r="P116" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K116" s="1" t="s">
+      <c r="Q116" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L116" s="1" t="s">
+      <c r="R116" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M116" s="1" t="s">
+      <c r="S116" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N116" s="1" t="s">
+      <c r="T116" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O116" s="1" t="s">
+      <c r="U116" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="V116" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W116" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X116" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y116" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z116" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA116" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>0.03</v>
       </c>
@@ -3353,29 +3953,29 @@
       <c r="G117" s="1">
         <v>14024</v>
       </c>
-      <c r="I117" s="1">
+      <c r="O117" s="10">
         <v>0</v>
       </c>
-      <c r="J117" s="4">
+      <c r="P117" s="10">
         <v>238</v>
       </c>
-      <c r="K117" s="4">
+      <c r="Q117" s="10">
         <v>234.02</v>
       </c>
-      <c r="L117" s="4">
+      <c r="R117" s="10">
         <v>228</v>
       </c>
-      <c r="M117" s="4">
+      <c r="S117" s="10">
         <v>1602</v>
       </c>
-      <c r="N117" s="4">
+      <c r="T117" s="10">
         <v>2100.3200000000002</v>
       </c>
-      <c r="O117" s="4">
+      <c r="U117" s="10">
         <v>13315</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>0.05</v>
       </c>
@@ -3397,29 +3997,29 @@
       <c r="G118" s="9">
         <v>14262</v>
       </c>
-      <c r="I118" s="1">
+      <c r="O118" s="1">
         <v>0.01</v>
       </c>
-      <c r="J118" s="4">
+      <c r="P118" s="4">
         <v>238</v>
       </c>
-      <c r="K118" s="4">
+      <c r="Q118" s="4">
         <v>232.2</v>
       </c>
-      <c r="L118" s="4">
+      <c r="R118" s="4">
         <v>226</v>
       </c>
-      <c r="M118" s="4">
+      <c r="S118" s="4">
         <v>1602</v>
       </c>
-      <c r="N118" s="4">
+      <c r="T118" s="4">
         <v>3164.58</v>
       </c>
-      <c r="O118" s="4">
+      <c r="U118" s="4">
         <v>13249</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -3441,29 +4041,29 @@
       <c r="G119" s="4">
         <v>14573</v>
       </c>
-      <c r="I119" s="1">
+      <c r="O119" s="1">
         <v>0.02</v>
       </c>
-      <c r="J119" s="4">
+      <c r="P119" s="4">
         <v>237</v>
       </c>
-      <c r="K119" s="4">
+      <c r="Q119" s="4">
         <v>230.22</v>
       </c>
-      <c r="L119" s="4">
+      <c r="R119" s="4">
         <v>225</v>
       </c>
-      <c r="M119" s="4">
+      <c r="S119" s="4">
         <v>1573</v>
       </c>
-      <c r="N119" s="4">
+      <c r="T119" s="4">
         <v>8011</v>
       </c>
-      <c r="O119" s="4">
+      <c r="U119" s="4">
         <v>14115</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>0.1</v>
       </c>
@@ -3485,29 +4085,29 @@
       <c r="G120" s="1">
         <v>14184</v>
       </c>
-      <c r="I120" s="1">
+      <c r="O120" s="1">
         <v>0.03</v>
       </c>
-      <c r="J120" s="4">
+      <c r="P120" s="4">
         <v>231</v>
       </c>
-      <c r="K120" s="4">
+      <c r="Q120" s="4">
         <v>227.02</v>
       </c>
-      <c r="L120" s="4">
+      <c r="R120" s="4">
         <v>225</v>
       </c>
-      <c r="M120" s="4">
+      <c r="S120" s="4">
         <v>1656</v>
       </c>
-      <c r="N120" s="4">
+      <c r="T120" s="4">
         <v>13007.54</v>
       </c>
-      <c r="O120" s="4">
+      <c r="U120" s="4">
         <v>16172</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>0.15</v>
       </c>
@@ -3529,54 +4129,54 @@
       <c r="G121" s="1">
         <v>15612</v>
       </c>
-      <c r="I121" s="1">
+      <c r="O121" s="1">
         <v>0.04</v>
       </c>
-      <c r="J121" s="4">
+      <c r="P121" s="4">
         <v>234</v>
       </c>
-      <c r="K121" s="4">
+      <c r="Q121" s="4">
         <v>226.42</v>
       </c>
-      <c r="L121" s="4">
+      <c r="R121" s="4">
         <v>225</v>
       </c>
-      <c r="M121" s="4">
+      <c r="S121" s="4">
         <v>1648</v>
       </c>
-      <c r="N121" s="4">
+      <c r="T121" s="4">
         <v>12852.58</v>
       </c>
-      <c r="O121" s="4">
+      <c r="U121" s="4">
         <v>16163</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>19</v>
       </c>
@@ -3599,7 +4199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>0</v>
       </c>
@@ -3621,8 +4221,26 @@
       <c r="G129" s="9">
         <v>13550</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H129" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>0.01</v>
       </c>
@@ -3645,7 +4263,7 @@
         <v>13475</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>0.02</v>
       </c>
@@ -3668,7 +4286,7 @@
         <v>13420</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>0.03</v>
       </c>
@@ -3691,7 +4309,7 @@
         <v>13402</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>0.04</v>
       </c>

</xml_diff>